<commit_message>
Gravando arquivo no banco de dados
</commit_message>
<xml_diff>
--- a/IApl-2019-1-SiglaProjeto/AS01/1.Documentos/Padrão para arquivo de texto.xlsx
+++ b/IApl-2019-1-SiglaProjeto/AS01/1.Documentos/Padrão para arquivo de texto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\IApl-2019-1\IApl-2019-1-SiglaProjeto\AS01\1.Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE59FEB0-6B71-4FED-AA66-880B8781FA81}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7188D065-D740-4068-837D-E6317BAB4C09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19740" yWindow="1620" windowWidth="15075" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -659,14 +659,14 @@
         <v>15</v>
       </c>
       <c r="D5" s="3">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E5" s="3">
         <v>140</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>

</xml_diff>